<commit_message>
End of analysis and coding
</commit_message>
<xml_diff>
--- a/Resources/nba_conf_wise.xlsx
+++ b/Resources/nba_conf_wise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99584ccd66595d1f/Documents/mathletics/NBA practice/nba21analysis/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_F25DC773A252ABDACC1048F0411A76785ADE58F1" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{242F7376-A8AB-4784-8DD5-5C153D64A02B}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC1048F0411A76785ADE58F1" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6F7BF344-50F5-4CA0-9BEB-363405741340}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,94 +58,94 @@
     <t>Western Conference</t>
   </si>
   <si>
-    <t>Philadelphia 76ers </t>
-  </si>
-  <si>
-    <t>Brooklyn Nets </t>
-  </si>
-  <si>
-    <t>Milwaukee Bucks </t>
-  </si>
-  <si>
-    <t>Atlanta Hawks </t>
-  </si>
-  <si>
-    <t>Miami Heat </t>
-  </si>
-  <si>
-    <t>Boston Celtics </t>
-  </si>
-  <si>
-    <t>New York Knicks </t>
-  </si>
-  <si>
-    <t>Charlotte Hornets </t>
-  </si>
-  <si>
-    <t>Indiana Pacers </t>
-  </si>
-  <si>
-    <t>Chicago Bulls </t>
-  </si>
-  <si>
-    <t>Toronto Raptors </t>
-  </si>
-  <si>
-    <t>Cleveland Cavaliers </t>
-  </si>
-  <si>
-    <t>Washington Wizards </t>
-  </si>
-  <si>
-    <t>Orlando Magic </t>
-  </si>
-  <si>
-    <t>Detroit Pistons </t>
-  </si>
-  <si>
-    <t>Utah Jazz </t>
-  </si>
-  <si>
-    <t>Phoenix Suns </t>
-  </si>
-  <si>
-    <t>Los Angeles Lakers </t>
-  </si>
-  <si>
-    <t>Los Angeles Clippers </t>
-  </si>
-  <si>
-    <t>Denver Nuggets </t>
-  </si>
-  <si>
-    <t>Portland Trail Blazers </t>
-  </si>
-  <si>
-    <t>San Antonio Spurs </t>
-  </si>
-  <si>
-    <t>Dallas Mavericks </t>
-  </si>
-  <si>
-    <t>Golden State Warriors </t>
-  </si>
-  <si>
-    <t>Memphis Grizzlies </t>
-  </si>
-  <si>
-    <t>New Orleans Pelicans </t>
-  </si>
-  <si>
-    <t>Oklahoma City Thunder </t>
-  </si>
-  <si>
-    <t>Sacramento Kings </t>
-  </si>
-  <si>
-    <t>Houston Rockets </t>
-  </si>
-  <si>
-    <t>Minnesota Timberwolves </t>
+    <t>Philadelphia 76ers (1) </t>
+  </si>
+  <si>
+    <t>Milwaukee Bucks (2) </t>
+  </si>
+  <si>
+    <t>Brooklyn Nets (3) </t>
+  </si>
+  <si>
+    <t>Charlotte Hornets (4) </t>
+  </si>
+  <si>
+    <t>Miami Heat (5) </t>
+  </si>
+  <si>
+    <t>New York Knicks (6) </t>
+  </si>
+  <si>
+    <t>Atlanta Hawks (7) </t>
+  </si>
+  <si>
+    <t>Boston Celtics (8) </t>
+  </si>
+  <si>
+    <t>Indiana Pacers (9) </t>
+  </si>
+  <si>
+    <t>Chicago Bulls (10) </t>
+  </si>
+  <si>
+    <t>Toronto Raptors (11) </t>
+  </si>
+  <si>
+    <t>Cleveland Cavaliers (12) </t>
+  </si>
+  <si>
+    <t>Washington Wizards (13) </t>
+  </si>
+  <si>
+    <t>Orlando Magic (14) </t>
+  </si>
+  <si>
+    <t>Detroit Pistons (15) </t>
+  </si>
+  <si>
+    <t>Utah Jazz (1) </t>
+  </si>
+  <si>
+    <t>Phoenix Suns (2) </t>
+  </si>
+  <si>
+    <t>Los Angeles Clippers (3) </t>
+  </si>
+  <si>
+    <t>Los Angeles Lakers (4) </t>
+  </si>
+  <si>
+    <t>Denver Nuggets (5) </t>
+  </si>
+  <si>
+    <t>Portland Trail Blazers (6) </t>
+  </si>
+  <si>
+    <t>Dallas Mavericks (7) </t>
+  </si>
+  <si>
+    <t>San Antonio Spurs (8) </t>
+  </si>
+  <si>
+    <t>Memphis Grizzlies (9) </t>
+  </si>
+  <si>
+    <t>Golden State Warriors (10) </t>
+  </si>
+  <si>
+    <t>New Orleans Pelicans (11) </t>
+  </si>
+  <si>
+    <t>Sacramento Kings (12) </t>
+  </si>
+  <si>
+    <t>Oklahoma City Thunder (13) </t>
+  </si>
+  <si>
+    <t>Houston Rockets (14) </t>
+  </si>
+  <si>
+    <t>Minnesota Timberwolves (15) </t>
   </si>
 </sst>
 </file>
@@ -208,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -321,12 +321,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF747678"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF747678"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF747678"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF747678"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF747678"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -352,9 +387,25 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -639,7 +690,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,25 +729,25 @@
         <v>10</v>
       </c>
       <c r="B2" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1">
         <v>13</v>
       </c>
       <c r="D2" s="1">
-        <v>0.69799999999999995</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="1">
-        <v>115.1</v>
+        <v>115</v>
       </c>
       <c r="G2" s="1">
-        <v>109.7</v>
+        <v>109.4</v>
       </c>
       <c r="H2" s="6">
-        <v>4.92</v>
+        <v>5.03</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -713,16 +764,16 @@
         <v>0.67400000000000004</v>
       </c>
       <c r="E3" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F3" s="1">
-        <v>120.2</v>
+        <v>120</v>
       </c>
       <c r="G3" s="1">
-        <v>115.2</v>
+        <v>112.6</v>
       </c>
       <c r="H3" s="6">
-        <v>4.42</v>
+        <v>6.99</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -730,25 +781,25 @@
         <v>12</v>
       </c>
       <c r="B4" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1">
-        <v>0.65900000000000003</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="E4" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F4" s="1">
-        <v>119.5</v>
+        <v>119.4</v>
       </c>
       <c r="G4" s="1">
-        <v>112.5</v>
+        <v>115.2</v>
       </c>
       <c r="H4" s="6">
-        <v>6.56</v>
+        <v>3.86</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -759,22 +810,22 @@
         <v>22</v>
       </c>
       <c r="C5" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1">
-        <v>0.52400000000000002</v>
+        <v>0.51200000000000001</v>
       </c>
       <c r="E5" s="1">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="F5" s="1">
-        <v>112.6</v>
+        <v>112</v>
       </c>
       <c r="G5" s="1">
-        <v>110.5</v>
+        <v>112.7</v>
       </c>
       <c r="H5" s="6">
-        <v>1.73</v>
+        <v>-0.83</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -785,22 +836,22 @@
         <v>22</v>
       </c>
       <c r="C6" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1">
-        <v>0.51200000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="E6" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1">
-        <v>106.3</v>
+        <v>106.2</v>
       </c>
       <c r="G6" s="1">
         <v>107.6</v>
       </c>
       <c r="H6" s="6">
-        <v>-1.24</v>
+        <v>-1.21</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -808,25 +859,25 @@
         <v>15</v>
       </c>
       <c r="B7" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1">
         <v>0.5</v>
       </c>
       <c r="E7" s="1">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1">
-        <v>111.7</v>
+        <v>105.3</v>
       </c>
       <c r="G7" s="1">
-        <v>110.8</v>
+        <v>105</v>
       </c>
       <c r="H7" s="6">
-        <v>1.08</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -834,25 +885,25 @@
         <v>16</v>
       </c>
       <c r="B8" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1">
         <v>22</v>
       </c>
       <c r="D8" s="1">
-        <v>0.48799999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="E8" s="1">
         <v>9</v>
       </c>
       <c r="F8" s="1">
-        <v>104.7</v>
+        <v>112.5</v>
       </c>
       <c r="G8" s="1">
-        <v>104.8</v>
+        <v>110.7</v>
       </c>
       <c r="H8" s="6">
-        <v>-0.63</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -860,25 +911,25 @@
         <v>17</v>
       </c>
       <c r="B9" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1">
-        <v>0.48799999999999999</v>
+        <v>0.47699999999999998</v>
       </c>
       <c r="E9" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F9" s="1">
-        <v>112</v>
+        <v>112.2</v>
       </c>
       <c r="G9" s="1">
-        <v>113.5</v>
+        <v>111.5</v>
       </c>
       <c r="H9" s="6">
-        <v>-1.36</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -886,25 +937,25 @@
         <v>18</v>
       </c>
       <c r="B10" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1">
-        <v>0.46300000000000002</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="E10" s="1">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="F10" s="1">
         <v>113.1</v>
       </c>
       <c r="G10" s="1">
-        <v>112.6</v>
+        <v>113.2</v>
       </c>
       <c r="H10" s="6">
-        <v>1.02</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -915,22 +966,22 @@
         <v>19</v>
       </c>
       <c r="C11" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1">
-        <v>0.46300000000000002</v>
+        <v>0.442</v>
       </c>
       <c r="E11" s="1">
-        <v>10</v>
+        <v>11.5</v>
       </c>
       <c r="F11" s="1">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G11" s="1">
-        <v>113.8</v>
+        <v>113.7</v>
       </c>
       <c r="H11" s="6">
-        <v>-0.36</v>
+        <v>-1.07</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -938,25 +989,25 @@
         <v>20</v>
       </c>
       <c r="B12" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1">
-        <v>0.40500000000000003</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="E12" s="1">
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="F12" s="1">
-        <v>112.3</v>
+        <v>112.5</v>
       </c>
       <c r="G12" s="1">
-        <v>112.3</v>
+        <v>112.4</v>
       </c>
       <c r="H12" s="6">
-        <v>-0.24</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -964,25 +1015,25 @@
         <v>21</v>
       </c>
       <c r="B13" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1">
-        <v>0.38100000000000001</v>
+        <v>0.38600000000000001</v>
       </c>
       <c r="E13" s="1">
-        <v>13.5</v>
+        <v>14</v>
       </c>
       <c r="F13" s="1">
         <v>104</v>
       </c>
       <c r="G13" s="1">
-        <v>111.8</v>
+        <v>111.5</v>
       </c>
       <c r="H13" s="6">
-        <v>-7.07</v>
+        <v>-6.97</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -993,22 +1044,22 @@
         <v>15</v>
       </c>
       <c r="C14" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" s="1">
-        <v>0.36599999999999999</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="E14" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F14" s="1">
         <v>114.9</v>
       </c>
       <c r="G14" s="1">
-        <v>120</v>
+        <v>120.2</v>
       </c>
       <c r="H14" s="6">
-        <v>-4.3600000000000003</v>
+        <v>-4.72</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1016,16 +1067,16 @@
         <v>23</v>
       </c>
       <c r="B15" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D15" s="1">
-        <v>0.33300000000000002</v>
+        <v>0.34100000000000003</v>
       </c>
       <c r="E15" s="1">
-        <v>15.5</v>
+        <v>16</v>
       </c>
       <c r="F15" s="1">
         <v>104.5</v>
@@ -1034,52 +1085,52 @@
         <v>111.3</v>
       </c>
       <c r="H15" s="6">
-        <v>-7.33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+        <v>-6.98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="11">
         <v>12</v>
       </c>
-      <c r="C16" s="1">
-        <v>30</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="E16" s="1">
-        <v>17.5</v>
-      </c>
-      <c r="F16" s="1">
-        <v>107.1</v>
-      </c>
-      <c r="G16" s="1">
-        <v>110.8</v>
-      </c>
-      <c r="H16" s="1">
-        <v>-3.14</v>
+      <c r="C16" s="11">
+        <v>31</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="E16" s="11">
+        <v>18.5</v>
+      </c>
+      <c r="F16" s="11">
+        <v>107.2</v>
+      </c>
+      <c r="G16" s="11">
+        <v>110.9</v>
+      </c>
+      <c r="H16" s="12">
+        <v>-3.15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.basketball-reference.com/teams/PHI/2021.html" xr:uid="{8BBEBCD4-8354-45A5-80D2-314082723A22}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://www.basketball-reference.com/teams/BRK/2021.html" xr:uid="{A51AD65A-ED25-49EC-B927-A275BA0E396B}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://www.basketball-reference.com/teams/MIL/2021.html" xr:uid="{F54C8090-BFD1-483F-BF60-36CF953DC7A0}"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://www.basketball-reference.com/teams/ATL/2021.html" xr:uid="{9D4463A8-AB53-433D-8D2A-1F6170BE01F0}"/>
-    <hyperlink ref="A6" r:id="rId5" display="https://www.basketball-reference.com/teams/MIA/2021.html" xr:uid="{CA0EC91E-CD83-4A64-AD75-1A78FF00DBE2}"/>
-    <hyperlink ref="A7" r:id="rId6" display="https://www.basketball-reference.com/teams/BOS/2021.html" xr:uid="{43656B89-32DA-47A8-B68B-49925A22C594}"/>
-    <hyperlink ref="A8" r:id="rId7" display="https://www.basketball-reference.com/teams/NYK/2021.html" xr:uid="{2B3F4DF7-5178-4702-8AAB-C0CE69A8D382}"/>
-    <hyperlink ref="A9" r:id="rId8" display="https://www.basketball-reference.com/teams/CHO/2021.html" xr:uid="{4AFC5B0D-6AC5-4585-BBCB-5151CF7CAE42}"/>
-    <hyperlink ref="A10" r:id="rId9" display="https://www.basketball-reference.com/teams/IND/2021.html" xr:uid="{6B29CD43-FC8C-4E2F-89CF-C4004EE419E2}"/>
-    <hyperlink ref="A11" r:id="rId10" display="https://www.basketball-reference.com/teams/CHI/2021.html" xr:uid="{DFF24CDD-A5E8-43AC-A3B2-C3662CC1EA2F}"/>
-    <hyperlink ref="A12" r:id="rId11" display="https://www.basketball-reference.com/teams/TOR/2021.html" xr:uid="{CA5F668C-C26A-49A0-8720-EE3F7CD45235}"/>
-    <hyperlink ref="A13" r:id="rId12" display="https://www.basketball-reference.com/teams/CLE/2021.html" xr:uid="{0A99BA95-F79F-4377-A8E5-D407254A8BEF}"/>
-    <hyperlink ref="A14" r:id="rId13" display="https://www.basketball-reference.com/teams/WAS/2021.html" xr:uid="{FF40F411-9CE8-4375-978B-4E3188A07E0B}"/>
-    <hyperlink ref="A15" r:id="rId14" display="https://www.basketball-reference.com/teams/ORL/2021.html" xr:uid="{4182B72C-5C95-4ABA-BBB4-B5C62261FC11}"/>
-    <hyperlink ref="A16" r:id="rId15" display="https://www.basketball-reference.com/teams/DET/2021.html" xr:uid="{DC5653AE-30BB-4425-9F30-601A3DA47D19}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.basketball-reference.com/teams/PHI/2021.html" xr:uid="{81289C88-50ED-4B60-92F0-FD1D4815F08F}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://www.basketball-reference.com/teams/MIL/2021.html" xr:uid="{9006AFB0-B317-45B4-9CF9-0487B706E317}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://www.basketball-reference.com/teams/BRK/2021.html" xr:uid="{2C8D0873-6597-441B-811F-EBE81C0216B4}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://www.basketball-reference.com/teams/CHO/2021.html" xr:uid="{43BB17F2-E071-4646-8D4E-AEE5C5A39963}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://www.basketball-reference.com/teams/MIA/2021.html" xr:uid="{049D36B8-463D-4003-AA18-A5E2C7EC3EF9}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://www.basketball-reference.com/teams/NYK/2021.html" xr:uid="{6224B524-89A0-4543-AB2D-BBCC72E0F0CA}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://www.basketball-reference.com/teams/ATL/2021.html" xr:uid="{17364650-E279-40AC-9DAB-386120561C14}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://www.basketball-reference.com/teams/BOS/2021.html" xr:uid="{216FA501-EC8A-4E0E-BE4F-DFF763C4D17B}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://www.basketball-reference.com/teams/IND/2021.html" xr:uid="{43B0589D-E483-4A8A-8C49-E747E85704E3}"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://www.basketball-reference.com/teams/CHI/2021.html" xr:uid="{C9CB1026-B7B2-41FD-AC87-20F3670F8B7B}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://www.basketball-reference.com/teams/TOR/2021.html" xr:uid="{D63C3C78-5E29-4B87-823D-71446ECA48BE}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://www.basketball-reference.com/teams/CLE/2021.html" xr:uid="{225FF83B-2AE4-4072-B62C-14C37F360715}"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://www.basketball-reference.com/teams/WAS/2021.html" xr:uid="{C7DCAF58-8C9A-4459-A88B-DA025F22E908}"/>
+    <hyperlink ref="A15" r:id="rId14" display="https://www.basketball-reference.com/teams/ORL/2021.html" xr:uid="{496715DF-A36F-41A7-8746-6BDB959FCBCA}"/>
+    <hyperlink ref="A16" r:id="rId15" display="https://www.basketball-reference.com/teams/DET/2021.html" xr:uid="{7BE3B384-40B7-40DB-930D-BA0FA6FC3BEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId16"/>
@@ -1091,7 +1142,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,28 +1151,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1130,25 +1181,25 @@
         <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1">
         <v>11</v>
       </c>
       <c r="D2" s="1">
-        <v>0.73199999999999998</v>
+        <v>0.74399999999999999</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="1">
-        <v>116.7</v>
+        <v>116.8</v>
       </c>
       <c r="G2" s="1">
-        <v>108.9</v>
+        <v>108</v>
       </c>
       <c r="H2" s="6">
-        <v>8.39</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1156,25 +1207,25 @@
         <v>26</v>
       </c>
       <c r="B3" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1">
-        <v>0.68300000000000005</v>
+        <v>0.67400000000000004</v>
       </c>
       <c r="E3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1">
-        <v>114.1</v>
+        <v>113.9</v>
       </c>
       <c r="G3" s="1">
-        <v>107.5</v>
+        <v>107.4</v>
       </c>
       <c r="H3" s="6">
-        <v>6.4</v>
+        <v>6.12</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1182,25 +1233,25 @@
         <v>27</v>
       </c>
       <c r="B4" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1">
-        <v>0.65100000000000002</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="E4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1">
-        <v>111.5</v>
+        <v>115.2</v>
       </c>
       <c r="G4" s="1">
-        <v>106.2</v>
+        <v>109.1</v>
       </c>
       <c r="H4" s="6">
-        <v>4.8099999999999996</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1208,25 +1259,25 @@
         <v>28</v>
       </c>
       <c r="B5" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1">
         <v>16</v>
       </c>
       <c r="D5" s="1">
-        <v>0.628</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="E5" s="1">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="F5" s="1">
-        <v>114.7</v>
+        <v>111.5</v>
       </c>
       <c r="G5" s="1">
-        <v>109.3</v>
+        <v>106.7</v>
       </c>
       <c r="H5" s="6">
-        <v>5.23</v>
+        <v>4.2300000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1234,25 +1285,25 @@
         <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1">
-        <v>0.59499999999999997</v>
+        <v>0.59099999999999997</v>
       </c>
       <c r="E6" s="1">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="F6" s="1">
-        <v>115.9</v>
+        <v>115.6</v>
       </c>
       <c r="G6" s="1">
-        <v>110.7</v>
+        <v>111</v>
       </c>
       <c r="H6" s="6">
-        <v>5.27</v>
+        <v>4.58</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1263,22 +1314,22 @@
         <v>25</v>
       </c>
       <c r="C7" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1">
-        <v>0.59499999999999997</v>
+        <v>0.58099999999999996</v>
       </c>
       <c r="E7" s="1">
-        <v>5.5</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1">
-        <v>114.5</v>
+        <v>114.4</v>
       </c>
       <c r="G7" s="1">
         <v>115.5</v>
       </c>
       <c r="H7" s="6">
-        <v>-1.55</v>
+        <v>-1.51</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1286,25 +1337,25 @@
         <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1">
-        <v>0.56399999999999995</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="E8" s="1">
-        <v>7</v>
+        <v>8.5</v>
       </c>
       <c r="F8" s="1">
-        <v>110.3</v>
+        <v>112.5</v>
       </c>
       <c r="G8" s="1">
-        <v>110.4</v>
+        <v>111.1</v>
       </c>
       <c r="H8" s="6">
-        <v>-0.78</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1321,16 +1372,16 @@
         <v>0.53700000000000003</v>
       </c>
       <c r="E9" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1">
-        <v>112.1</v>
+        <v>109.8</v>
       </c>
       <c r="G9" s="1">
-        <v>111.1</v>
+        <v>110.7</v>
       </c>
       <c r="H9" s="6">
-        <v>1.8</v>
+        <v>-1.49</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1338,25 +1389,25 @@
         <v>33</v>
       </c>
       <c r="B10" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1">
         <v>0.51200000000000001</v>
       </c>
       <c r="E10" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1">
-        <v>112.9</v>
+        <v>111.5</v>
       </c>
       <c r="G10" s="1">
-        <v>113.1</v>
+        <v>110.9</v>
       </c>
       <c r="H10" s="6">
-        <v>0.3</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1364,25 +1415,25 @@
         <v>34</v>
       </c>
       <c r="B11" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1">
-        <v>0.48699999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="E11" s="1">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="F11" s="1">
-        <v>110.9</v>
+        <v>112.5</v>
       </c>
       <c r="G11" s="1">
-        <v>110.6</v>
+        <v>113</v>
       </c>
       <c r="H11" s="6">
-        <v>0.41</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1390,25 +1441,25 @@
         <v>35</v>
       </c>
       <c r="B12" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1">
         <v>24</v>
       </c>
       <c r="D12" s="1">
-        <v>0.42899999999999999</v>
+        <v>0.442</v>
       </c>
       <c r="E12" s="1">
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="F12" s="1">
-        <v>115.3</v>
+        <v>115.6</v>
       </c>
       <c r="G12" s="1">
-        <v>115.2</v>
+        <v>115.1</v>
       </c>
       <c r="H12" s="6">
-        <v>0.25</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1416,25 +1467,25 @@
         <v>36</v>
       </c>
       <c r="B13" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" s="1">
-        <v>0.42899999999999999</v>
+        <v>0.432</v>
       </c>
       <c r="E13" s="1">
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
       <c r="F13" s="1">
-        <v>106.2</v>
+        <v>114.5</v>
       </c>
       <c r="G13" s="1">
-        <v>112.2</v>
+        <v>119</v>
       </c>
       <c r="H13" s="6">
-        <v>-5.55</v>
+        <v>-4.12</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1442,25 +1493,25 @@
         <v>37</v>
       </c>
       <c r="B14" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1">
         <v>25</v>
       </c>
       <c r="D14" s="1">
-        <v>0.40500000000000003</v>
+        <v>0.432</v>
       </c>
       <c r="E14" s="1">
         <v>13.5</v>
       </c>
       <c r="F14" s="1">
-        <v>114.5</v>
+        <v>106.4</v>
       </c>
       <c r="G14" s="1">
-        <v>119.6</v>
+        <v>112</v>
       </c>
       <c r="H14" s="6">
-        <v>-4.5599999999999996</v>
+        <v>-5.51</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1468,25 +1519,25 @@
         <v>38</v>
       </c>
       <c r="B15" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D15" s="1">
-        <v>0.26800000000000002</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="E15" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F15" s="1">
         <v>106.9</v>
       </c>
       <c r="G15" s="1">
-        <v>113.7</v>
+        <v>113.6</v>
       </c>
       <c r="H15" s="6">
-        <v>-7.57</v>
+        <v>-7.45</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1497,41 +1548,41 @@
         <v>10</v>
       </c>
       <c r="C16" s="8">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D16" s="8">
-        <v>0.23799999999999999</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="E16" s="8">
-        <v>20.5</v>
+        <v>22.5</v>
       </c>
       <c r="F16" s="8">
-        <v>109.5</v>
+        <v>109.3</v>
       </c>
       <c r="G16" s="8">
-        <v>117.2</v>
-      </c>
-      <c r="H16" s="9">
-        <v>-7</v>
+        <v>117.3</v>
+      </c>
+      <c r="H16" s="15">
+        <v>-7.52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.basketball-reference.com/teams/UTA/2021.html" xr:uid="{40501281-3603-44B9-9962-67AA03138014}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://www.basketball-reference.com/teams/PHO/2021.html" xr:uid="{8A7180D2-1256-46B5-9D7C-F6900AC1D3A2}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://www.basketball-reference.com/teams/LAL/2021.html" xr:uid="{AC0ECDD6-830A-4621-8A44-1C3DD16A3A68}"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://www.basketball-reference.com/teams/LAC/2021.html" xr:uid="{3F3DEBD2-7F13-4962-BDD5-C1149F1EA63B}"/>
-    <hyperlink ref="A6" r:id="rId5" display="https://www.basketball-reference.com/teams/DEN/2021.html" xr:uid="{CD1484C9-FDD4-419A-B825-CCFAE5AE0910}"/>
-    <hyperlink ref="A7" r:id="rId6" display="https://www.basketball-reference.com/teams/POR/2021.html" xr:uid="{F9ACC245-5CC0-45D4-BBC5-A37E30934973}"/>
-    <hyperlink ref="A8" r:id="rId7" display="https://www.basketball-reference.com/teams/SAS/2021.html" xr:uid="{951CAE06-6FA5-4FE9-AF58-86BCC10AF2AA}"/>
-    <hyperlink ref="A9" r:id="rId8" display="https://www.basketball-reference.com/teams/DAL/2021.html" xr:uid="{4BCC54D4-AC18-471A-A21A-9F7522703234}"/>
-    <hyperlink ref="A10" r:id="rId9" display="https://www.basketball-reference.com/teams/GSW/2021.html" xr:uid="{1C25664A-D17C-4FF9-9F7B-31AC544D92CE}"/>
-    <hyperlink ref="A11" r:id="rId10" display="https://www.basketball-reference.com/teams/MEM/2021.html" xr:uid="{0BF2FE8D-C7B3-4EB5-8F21-00AAE99CCDB5}"/>
-    <hyperlink ref="A12" r:id="rId11" display="https://www.basketball-reference.com/teams/NOP/2021.html" xr:uid="{8C5D240A-633A-404F-A8DE-CABB8FCCC4EC}"/>
-    <hyperlink ref="A13" r:id="rId12" display="https://www.basketball-reference.com/teams/OKC/2021.html" xr:uid="{D9104F1B-5D22-46C0-AEDF-5F96086DF790}"/>
-    <hyperlink ref="A14" r:id="rId13" display="https://www.basketball-reference.com/teams/SAC/2021.html" xr:uid="{9A0CE4DE-DF89-4BB1-9612-8213EE9F086A}"/>
-    <hyperlink ref="A15" r:id="rId14" display="https://www.basketball-reference.com/teams/HOU/2021.html" xr:uid="{8B7EEE1A-9039-4CCD-A568-D845D30296DC}"/>
-    <hyperlink ref="A16" r:id="rId15" display="https://www.basketball-reference.com/teams/MIN/2021.html" xr:uid="{62B71A48-9ADE-4791-8603-2806310DC552}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.basketball-reference.com/teams/UTA/2021.html" xr:uid="{9BD9C723-7F17-4F69-BCEB-776ACA45F253}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://www.basketball-reference.com/teams/PHO/2021.html" xr:uid="{F6CE0406-0746-4912-8C42-8CEF1CC61448}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://www.basketball-reference.com/teams/LAC/2021.html" xr:uid="{35E51A10-B76C-435A-8DC9-5B87C0B601C2}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://www.basketball-reference.com/teams/LAL/2021.html" xr:uid="{57DDD8F5-8E0B-4AB8-878D-E32E73EF87B1}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://www.basketball-reference.com/teams/DEN/2021.html" xr:uid="{9FD2C77D-6F6A-4235-9ADB-BA2351B41766}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://www.basketball-reference.com/teams/POR/2021.html" xr:uid="{8AFC1758-5891-4055-B317-6239038104F4}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://www.basketball-reference.com/teams/DAL/2021.html" xr:uid="{06F75B35-6DCF-4ED4-920B-1DADDEDD6F4F}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://www.basketball-reference.com/teams/SAS/2021.html" xr:uid="{EA7FEC16-3D45-4E52-AC2C-53CED48CB966}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://www.basketball-reference.com/teams/MEM/2021.html" xr:uid="{919075F9-898E-4AD5-B507-FA236BA73F68}"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://www.basketball-reference.com/teams/GSW/2021.html" xr:uid="{0F8902AA-C177-4CB0-8CD3-67ADCDD52D78}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://www.basketball-reference.com/teams/NOP/2021.html" xr:uid="{543CBFC1-42F3-4B2A-8776-F92085FD8409}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://www.basketball-reference.com/teams/SAC/2021.html" xr:uid="{8F782C67-834E-43C4-9934-F44FFD776CFB}"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://www.basketball-reference.com/teams/OKC/2021.html" xr:uid="{6CFDD7DB-03C8-4FDE-9D4A-FD61C8C3BA68}"/>
+    <hyperlink ref="A15" r:id="rId14" display="https://www.basketball-reference.com/teams/HOU/2021.html" xr:uid="{BA29E463-ED3A-4A36-BA38-B1CB72D5DAB9}"/>
+    <hyperlink ref="A16" r:id="rId15" display="https://www.basketball-reference.com/teams/MIN/2021.html" xr:uid="{7176F076-7BD1-48B3-B091-5C847EB148DC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>